<commit_message>
Files used in ZEV analysis and ZEV + CES + building electrification analysis
</commit_message>
<xml_diff>
--- a/InputData/ccs/CPbE/CCS Percentages by Entity.xlsx
+++ b/InputData/ccs/CPbE/CCS Percentages by Entity.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-california\InputData\ccs\CPbE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="18960" windowHeight="7163"/>
   </bookViews>
@@ -13,7 +18,7 @@
     <sheet name="CPbE-FoESCbES" sheetId="5" r:id="rId4"/>
     <sheet name="CPbE-PoICbI" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -236,7 +241,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
@@ -308,6 +313,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -355,7 +363,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,7 +398,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2507,7 +2515,7 @@
   <dimension ref="A1:AM3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2639,156 +2647,118 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
@@ -2796,156 +2766,155 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <f>About!$I$23</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <f>$B$3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:AM3" si="0">$B$3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2961,7 +2930,7 @@
   <dimension ref="A1:AM14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B14" sqref="B14:AM14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3093,155 +3062,117 @@
         <v>32</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:D14" si="0">C2</f>
-        <v>5.9005721409314106E-4</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <f t="shared" si="0"/>
-        <v>5.9005721409314106E-4</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <f t="shared" si="0"/>
-        <v>5.9005721409314106E-4</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <f>F2</f>
-        <v>5.9005721409314106E-4</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <f>'Technologies to power CCS'!B19</f>
-        <v>5.9005721409314106E-4</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <f>'Technologies to power CCS'!C19</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f>'Technologies to power CCS'!D19</f>
         <v>0</v>
       </c>
       <c r="I2">
-        <f>'Technologies to power CCS'!E19</f>
         <v>0</v>
       </c>
       <c r="J2">
-        <f>'Technologies to power CCS'!F19</f>
         <v>0</v>
       </c>
       <c r="K2">
-        <f>'Technologies to power CCS'!G19</f>
         <v>0</v>
       </c>
       <c r="L2">
-        <f>'Technologies to power CCS'!H19</f>
         <v>0</v>
       </c>
       <c r="M2">
-        <f>'Technologies to power CCS'!I19</f>
         <v>0</v>
       </c>
       <c r="N2">
-        <f>'Technologies to power CCS'!J19</f>
         <v>0</v>
       </c>
       <c r="O2">
-        <f>'Technologies to power CCS'!K19</f>
         <v>0</v>
       </c>
       <c r="P2">
-        <f>'Technologies to power CCS'!L19</f>
         <v>0</v>
       </c>
       <c r="Q2">
-        <f>'Technologies to power CCS'!M19</f>
         <v>0</v>
       </c>
       <c r="R2">
-        <f>'Technologies to power CCS'!N19</f>
         <v>0</v>
       </c>
       <c r="S2">
-        <f>'Technologies to power CCS'!O19</f>
         <v>0</v>
       </c>
       <c r="T2">
-        <f>S2</f>
         <v>0</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:AM14" si="1">T2</f>
         <v>0</v>
       </c>
       <c r="V2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3250,156 +3181,118 @@
         <v>26</v>
       </c>
       <c r="B3">
-        <f t="shared" si="0"/>
-        <v>0.3335464691512724</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
-        <v>0.3335464691512724</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
-        <v>0.3335464691512724</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E14" si="2">F3</f>
-        <v>0.3335464691512724</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <f>'Technologies to power CCS'!B20</f>
-        <v>0.3335464691512724</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <f>'Technologies to power CCS'!C20</f>
-        <v>0.30616347531420662</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <f>'Technologies to power CCS'!D20</f>
-        <v>0.28003302126930857</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <f>'Technologies to power CCS'!E20</f>
-        <v>0.25791944378357839</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <f>'Technologies to power CCS'!F20</f>
-        <v>0.24105755214185653</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <f>'Technologies to power CCS'!G20</f>
-        <v>0.22761293681353043</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <f>'Technologies to power CCS'!H20</f>
-        <v>0.21576323530147837</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <f>'Technologies to power CCS'!I20</f>
-        <v>0.20459795910285011</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <f>'Technologies to power CCS'!J20</f>
-        <v>0.19296502094063003</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <f>'Technologies to power CCS'!K20</f>
-        <v>0.1865838936388145</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <f>'Technologies to power CCS'!L20</f>
-        <v>0.18044668164628119</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <f>'Technologies to power CCS'!M20</f>
-        <v>0.17592139040828728</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <f>'Technologies to power CCS'!N20</f>
-        <v>0.1707093578327098</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <f>'Technologies to power CCS'!O20</f>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:AI14" si="3">S3</f>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="U3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="Y3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="Z3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AA3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AB3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AC3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AD3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AE3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AF3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AG3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AH3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AI3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AJ3">
-        <f t="shared" si="1"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AK3">
-        <f t="shared" si="1"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AL3">
-        <f t="shared" si="1"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AM3">
-        <f t="shared" si="1"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
@@ -3407,155 +3300,117 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>2.5672852969543393E-2</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>2.5672852969543393E-2</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>2.5672852969543393E-2</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="2"/>
-        <v>2.5672852969543393E-2</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <f>'Technologies to power CCS'!B21</f>
-        <v>2.5672852969543393E-2</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <f>'Technologies to power CCS'!C21</f>
-        <v>2.3627823761908948E-2</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <f>'Technologies to power CCS'!D21</f>
-        <v>2.2271673465437025E-2</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <f>'Technologies to power CCS'!E21</f>
-        <v>2.1243390846433275E-2</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <f>'Technologies to power CCS'!F21</f>
-        <v>2.0604460654779281E-2</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <f>'Technologies to power CCS'!G21</f>
-        <v>2.0224335461973515E-2</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <f>'Technologies to power CCS'!H21</f>
-        <v>1.9962860570305472E-2</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <f>'Technologies to power CCS'!I21</f>
-        <v>1.9743963776055761E-2</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <f>'Technologies to power CCS'!J21</f>
         <v>0</v>
       </c>
       <c r="O4">
-        <f>'Technologies to power CCS'!K21</f>
         <v>0</v>
       </c>
       <c r="P4">
-        <f>'Technologies to power CCS'!L21</f>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f>'Technologies to power CCS'!M21</f>
         <v>0</v>
       </c>
       <c r="R4">
-        <f>'Technologies to power CCS'!N21</f>
         <v>0</v>
       </c>
       <c r="S4">
-        <f>'Technologies to power CCS'!O21</f>
         <v>0</v>
       </c>
       <c r="T4">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3564,156 +3419,118 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>0.15011055526529507</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>0.15011055526529507</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0.15011055526529507</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
-        <v>0.15011055526529507</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <f>'Technologies to power CCS'!B22</f>
-        <v>0.15011055526529507</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <f>'Technologies to power CCS'!C22</f>
-        <v>0.13815315924639782</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <f>'Technologies to power CCS'!D22</f>
-        <v>0.13022367535662133</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <f>'Technologies to power CCS'!E22</f>
-        <v>0.12421125145143937</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <f>'Technologies to power CCS'!F22</f>
-        <v>0.12047539217788203</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <f>'Technologies to power CCS'!G22</f>
-        <v>0.11825277968405075</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <f>'Technologies to power CCS'!H22</f>
-        <v>0.11672392189708072</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <f>'Technologies to power CCS'!I22</f>
-        <v>0.11544402054098295</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <f>'Technologies to power CCS'!J22</f>
-        <v>0.11369860119516798</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <f>'Technologies to power CCS'!K22</f>
-        <v>0.11032899203363489</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <f>'Technologies to power CCS'!L22</f>
-        <v>0.10759484910422214</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <f>'Technologies to power CCS'!M22</f>
-        <v>0.10576827133280721</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <f>'Technologies to power CCS'!N22</f>
-        <v>0.10354767722253042</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <f>'Technologies to power CCS'!O22</f>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <f t="shared" si="3"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="U5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="V5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="W5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="X5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="Z5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AA5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AB5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AC5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AD5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AE5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AF5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AG5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AH5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AI5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AJ5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AK5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AL5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AM5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
@@ -3721,156 +3538,118 @@
         <v>33</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>9.0546961580838373E-2</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>9.0546961580838373E-2</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>9.0546961580838373E-2</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
-        <v>9.0546961580838373E-2</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <f>'Technologies to power CCS'!B23</f>
-        <v>9.0546961580838373E-2</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <f>'Technologies to power CCS'!C23</f>
-        <v>0.10313105691313788</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <f>'Technologies to power CCS'!D23</f>
-        <v>0.11442968042521866</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <f>'Technologies to power CCS'!E23</f>
-        <v>0.12312822024238593</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <f>'Technologies to power CCS'!F23</f>
-        <v>0.12713115819800086</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <f>'Technologies to power CCS'!G23</f>
-        <v>0.12951857123056587</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <f>'Technologies to power CCS'!H23</f>
-        <v>0.13076382759696545</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <f>'Technologies to power CCS'!I23</f>
-        <v>0.13164017636730868</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <f>'Technologies to power CCS'!J23</f>
-        <v>0.14106687512493682</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <f>'Technologies to power CCS'!K23</f>
-        <v>0.14315486351991433</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <f>'Technologies to power CCS'!L23</f>
-        <v>0.14445177533038972</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <f>'Technologies to power CCS'!M23</f>
-        <v>0.14676179158994082</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <f>'Technologies to power CCS'!N23</f>
-        <v>0.15008196784397632</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <f>'Technologies to power CCS'!O23</f>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <f t="shared" si="3"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="U6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="X6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="Z6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AA6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AC6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AD6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AE6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AF6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AG6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AH6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AI6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AJ6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AK6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AL6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AM6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
@@ -3878,156 +3657,118 @@
         <v>23</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>0.20936302787322997</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>0.20936302787322997</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>0.20936302787322997</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
-        <v>0.20936302787322997</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <f>'Technologies to power CCS'!B24</f>
-        <v>0.20936302787322997</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <f>'Technologies to power CCS'!C24</f>
-        <v>0.253754730748458</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <f>'Technologies to power CCS'!D24</f>
-        <v>0.28778669079043501</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <f>'Technologies to power CCS'!E24</f>
-        <v>0.31689315630803538</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <f>'Technologies to power CCS'!F24</f>
-        <v>0.33883704050029317</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <f>'Technologies to power CCS'!G24</f>
-        <v>0.35529923226968935</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <f>'Technologies to power CCS'!H24</f>
-        <v>0.36962158157910979</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <f>'Technologies to power CCS'!I24</f>
-        <v>0.38302299639608717</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <f>'Technologies to power CCS'!J24</f>
-        <v>0.4089192294628245</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <f>'Technologies to power CCS'!K24</f>
-        <v>0.42083035340445213</v>
+        <v>0</v>
       </c>
       <c r="P7">
-        <f>'Technologies to power CCS'!L24</f>
-        <v>0.4318519817230248</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <f>'Technologies to power CCS'!M24</f>
-        <v>0.44571287754404737</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <f>'Technologies to power CCS'!N24</f>
-        <v>0.4598258397929757</v>
+        <v>0</v>
       </c>
       <c r="S7">
-        <f>'Technologies to power CCS'!O24</f>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="T7">
-        <f t="shared" si="3"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="U7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="V7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="W7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="X7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AD7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AE7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AF7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AG7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AH7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AI7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AJ7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AK7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AL7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AM7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
@@ -4035,156 +3776,118 @@
         <v>24</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>1.3399662916406058E-2</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>1.3399662916406058E-2</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1.3399662916406058E-2</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
-        <v>1.3399662916406058E-2</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <f>'Technologies to power CCS'!B25</f>
-        <v>1.3399662916406058E-2</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <f>'Technologies to power CCS'!C25</f>
-        <v>1.2332282439876422E-2</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <f>'Technologies to power CCS'!D25</f>
-        <v>1.1624454725587482E-2</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <f>'Technologies to power CCS'!E25</f>
-        <v>1.1087753935309303E-2</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <f>'Technologies to power CCS'!F25</f>
-        <v>1.0754271357216599E-2</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <f>'Technologies to power CCS'!G25</f>
-        <v>1.0555869198497669E-2</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <f>'Technologies to power CCS'!H25</f>
-        <v>1.0419395257965539E-2</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <f>'Technologies to power CCS'!I25</f>
-        <v>1.0305144486541431E-2</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <f>'Technologies to power CCS'!J25</f>
-        <v>1.0149339114691595E-2</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <f>'Technologies to power CCS'!K25</f>
-        <v>9.8485499606925375E-3</v>
+        <v>0</v>
       </c>
       <c r="P8">
-        <f>'Technologies to power CCS'!L25</f>
-        <v>9.6044858870192578E-3</v>
+        <v>0</v>
       </c>
       <c r="Q8">
-        <f>'Technologies to power CCS'!M25</f>
-        <v>9.4414358844108204E-3</v>
+        <v>0</v>
       </c>
       <c r="R8">
-        <f>'Technologies to power CCS'!N25</f>
-        <v>9.2432138972942026E-3</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <f>'Technologies to power CCS'!O25</f>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="T8">
-        <f t="shared" si="3"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="U8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="V8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="W8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="X8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AA8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AB8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AD8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AE8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AF8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AG8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AH8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AI8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AJ8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AK8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AL8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AM8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
@@ -4192,156 +3895,118 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>1.4204286390169431E-2</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>1.4204286390169431E-2</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>1.4204286390169431E-2</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
-        <v>1.4204286390169431E-2</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <f>'Technologies to power CCS'!B26</f>
-        <v>1.4204286390169431E-2</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <f>'Technologies to power CCS'!C26</f>
-        <v>1.3072811809764917E-2</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <f>'Technologies to power CCS'!D26</f>
-        <v>1.2322480429686009E-2</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <f>'Technologies to power CCS'!E26</f>
-        <v>1.1753551809727395E-2</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <f>'Technologies to power CCS'!F26</f>
-        <v>1.1400044256969397E-2</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <f>'Technologies to power CCS'!G26</f>
-        <v>1.118972843779897E-2</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <f>'Technologies to power CCS'!H26</f>
-        <v>1.1045059504840972E-2</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <f>'Technologies to power CCS'!I26</f>
-        <v>1.0923948198703647E-2</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <f>'Technologies to power CCS'!J26</f>
-        <v>1.0758787019897256E-2</v>
+        <v>0</v>
       </c>
       <c r="O9">
-        <f>'Technologies to power CCS'!K26</f>
-        <v>1.043993606721931E-2</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <f>'Technologies to power CCS'!L26</f>
-        <v>1.0181216424670533E-2</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <f>'Technologies to power CCS'!M26</f>
-        <v>1.0008375589239333E-2</v>
+        <v>0</v>
       </c>
       <c r="R9">
-        <f>'Technologies to power CCS'!N26</f>
-        <v>9.7982507606225178E-3</v>
+        <v>0</v>
       </c>
       <c r="S9">
-        <f>'Technologies to power CCS'!O26</f>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="T9">
-        <f t="shared" si="3"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="U9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="V9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="W9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AB9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AD9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AE9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AF9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AG9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AH9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AI9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AJ9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AK9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AL9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AM9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
@@ -4349,156 +4014,118 @@
         <v>27</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>2.9116641437250634E-2</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>2.9116641437250634E-2</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>2.9116641437250634E-2</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
-        <v>2.9116641437250634E-2</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <f>'Technologies to power CCS'!B27</f>
-        <v>2.9116641437250634E-2</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <f>'Technologies to power CCS'!C27</f>
-        <v>2.6896026714350176E-2</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <f>'Technologies to power CCS'!D27</f>
-        <v>2.5445363666738333E-2</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <f>'Technologies to power CCS'!E27</f>
-        <v>2.4359324898709948E-2</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <f>'Technologies to power CCS'!F27</f>
-        <v>2.3626677825622375E-2</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <f>'Technologies to power CCS'!G27</f>
-        <v>2.3190796701903604E-2</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <f>'Technologies to power CCS'!H27</f>
-        <v>2.2890969245682499E-2</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <f>'Technologies to power CCS'!I27</f>
-        <v>2.2639965148974931E-2</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <f>'Technologies to power CCS'!J27</f>
-        <v>2.2297667358457757E-2</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <f>'Technologies to power CCS'!K27</f>
-        <v>2.1636846350792893E-2</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <f>'Technologies to power CCS'!L27</f>
-        <v>2.1100647937534699E-2</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <f>'Technologies to power CCS'!M27</f>
-        <v>2.0742434000659161E-2</v>
+        <v>0</v>
       </c>
       <c r="R10">
-        <f>'Technologies to power CCS'!N27</f>
-        <v>2.0306948706305276E-2</v>
+        <v>0</v>
       </c>
       <c r="S10">
-        <f>'Technologies to power CCS'!O27</f>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="T10">
-        <f t="shared" si="3"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="U10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="V10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="W10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="X10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AB10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AD10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AE10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AF10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AH10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AI10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AJ10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AK10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AL10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AM10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
@@ -4506,156 +4133,118 @@
         <v>28</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
-        <v>3.8085511091466378E-3</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>3.8085511091466378E-3</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>3.8085511091466378E-3</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
-        <v>3.8085511091466378E-3</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <f>'Technologies to power CCS'!B28</f>
-        <v>3.8085511091466378E-3</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <f>'Technologies to power CCS'!C28</f>
-        <v>3.5051723508055482E-3</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <f>'Technologies to power CCS'!D28</f>
-        <v>3.3039883327330316E-3</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <f>'Technologies to power CCS'!E28</f>
-        <v>3.1514432722456387E-3</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <f>'Technologies to power CCS'!F28</f>
-        <v>3.0566583921632444E-3</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <f>'Technologies to power CCS'!G28</f>
-        <v>3.000267066026159E-3</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <f>'Technologies to power CCS'!H28</f>
-        <v>2.9614774352103817E-3</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <f>'Technologies to power CCS'!I28</f>
-        <v>2.9290042375678207E-3</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <f>'Technologies to power CCS'!J28</f>
-        <v>2.8847200846401251E-3</v>
+        <v>0</v>
       </c>
       <c r="O11">
-        <f>'Technologies to power CCS'!K28</f>
-        <v>2.7992275708933951E-3</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <f>'Technologies to power CCS'!L28</f>
-        <v>2.729857878216042E-3</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <f>'Technologies to power CCS'!M28</f>
-        <v>2.6835146028549571E-3</v>
+        <v>0</v>
       </c>
       <c r="R11">
-        <f>'Technologies to power CCS'!N28</f>
-        <v>2.6271744864206901E-3</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <f>'Technologies to power CCS'!O28</f>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="T11">
-        <f t="shared" si="3"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="U11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="V11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="W11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="X11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AD11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AE11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AF11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AH11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AI11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AJ11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AK11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AL11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AM11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
@@ -4663,156 +4252,118 @@
         <v>29</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
-        <v>0.12953365096291972</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>0.12953365096291972</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0.12953365096291972</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
-        <v>0.12953365096291972</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <f>'Technologies to power CCS'!B29</f>
-        <v>0.12953365096291972</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <f>'Technologies to power CCS'!C29</f>
-        <v>0.11921535482711602</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <f>'Technologies to power CCS'!D29</f>
-        <v>0.11237283135047499</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <f>'Technologies to power CCS'!E29</f>
-        <v>0.10603053082732931</v>
+        <v>1</v>
       </c>
       <c r="J12">
-        <f>'Technologies to power CCS'!F29</f>
-        <v>0.10284148686196562</v>
+        <v>1</v>
       </c>
       <c r="K12">
-        <f>'Technologies to power CCS'!G29</f>
-        <v>0.10094419672286321</v>
+        <v>1</v>
       </c>
       <c r="L12">
-        <f>'Technologies to power CCS'!H29</f>
-        <v>9.9639116862402247E-2</v>
+        <v>1</v>
       </c>
       <c r="M12">
-        <f>'Technologies to power CCS'!I29</f>
-        <v>9.854655384087338E-2</v>
+        <v>1</v>
       </c>
       <c r="N12">
-        <f>'Technologies to power CCS'!J29</f>
-        <v>9.7056610397018739E-2</v>
+        <v>1</v>
       </c>
       <c r="O12">
-        <f>'Technologies to power CCS'!K29</f>
-        <v>9.4180208751410463E-2</v>
+        <v>1</v>
       </c>
       <c r="P12">
-        <f>'Technologies to power CCS'!L29</f>
-        <v>9.1846260556091283E-2</v>
+        <v>1</v>
       </c>
       <c r="Q12">
-        <f>'Technologies to power CCS'!M29</f>
-        <v>8.2770929146143452E-2</v>
+        <v>1</v>
       </c>
       <c r="R12">
-        <f>'Technologies to power CCS'!N29</f>
-        <v>7.3674557169388963E-2</v>
+        <v>1</v>
       </c>
       <c r="S12">
-        <f>'Technologies to power CCS'!O29</f>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="T12">
-        <f t="shared" si="3"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="U12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="V12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="W12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="X12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AB12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AD12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AE12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AF12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AG12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AH12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AI12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AJ12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AK12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AL12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AM12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
@@ -4820,155 +4371,155 @@
         <v>30</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B2:D14" si="0">C13</f>
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C13:C14" si="1">D13</f>
         <v>0</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D13:D14" si="2">E13</f>
         <v>0</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E13:E14" si="3">F13</f>
         <v>0</v>
       </c>
       <c r="F13">
-        <f>'Technologies to power CCS'!B30</f>
+        <f t="shared" ref="F13:F14" si="4">G13</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <f>'Technologies to power CCS'!C30</f>
+        <f t="shared" ref="G13:G14" si="5">H13</f>
         <v>0</v>
       </c>
       <c r="H13">
-        <f>'Technologies to power CCS'!D30</f>
+        <f t="shared" ref="H13:H14" si="6">I13</f>
         <v>0</v>
       </c>
       <c r="I13">
-        <f>'Technologies to power CCS'!E30</f>
+        <f t="shared" ref="I13:I14" si="7">J13</f>
         <v>0</v>
       </c>
       <c r="J13">
-        <f>'Technologies to power CCS'!F30</f>
+        <f t="shared" ref="J13:J14" si="8">K13</f>
         <v>0</v>
       </c>
       <c r="K13">
-        <f>'Technologies to power CCS'!G30</f>
+        <f t="shared" ref="K13:K14" si="9">L13</f>
         <v>0</v>
       </c>
       <c r="L13">
-        <f>'Technologies to power CCS'!H30</f>
+        <f t="shared" ref="L13:L14" si="10">M13</f>
         <v>0</v>
       </c>
       <c r="M13">
-        <f>'Technologies to power CCS'!I30</f>
+        <f t="shared" ref="M13:M14" si="11">N13</f>
         <v>0</v>
       </c>
       <c r="N13">
-        <f>'Technologies to power CCS'!J30</f>
+        <f t="shared" ref="N13:N14" si="12">O13</f>
         <v>0</v>
       </c>
       <c r="O13">
-        <f>'Technologies to power CCS'!K30</f>
+        <f t="shared" ref="O13:O14" si="13">P13</f>
         <v>0</v>
       </c>
       <c r="P13">
-        <f>'Technologies to power CCS'!L30</f>
+        <f t="shared" ref="P13:P14" si="14">Q13</f>
         <v>0</v>
       </c>
       <c r="Q13">
-        <f>'Technologies to power CCS'!M30</f>
+        <f t="shared" ref="Q13:Q14" si="15">R13</f>
         <v>0</v>
       </c>
       <c r="R13">
-        <f>'Technologies to power CCS'!N30</f>
+        <f t="shared" ref="R13:R14" si="16">S13</f>
         <v>0</v>
       </c>
       <c r="S13">
-        <f>'Technologies to power CCS'!O30</f>
+        <f t="shared" ref="S13:S14" si="17">T13</f>
         <v>0</v>
       </c>
       <c r="T13">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="T13:T14" si="18">U13</f>
         <v>0</v>
       </c>
       <c r="U13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="U13:U14" si="19">V13</f>
         <v>0</v>
       </c>
       <c r="V13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="V13:V14" si="20">W13</f>
         <v>0</v>
       </c>
       <c r="W13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="W13:W14" si="21">X13</f>
         <v>0</v>
       </c>
       <c r="X13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="X13:X14" si="22">Y13</f>
         <v>0</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Y13:Y14" si="23">Z13</f>
         <v>0</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Z13:Z14" si="24">AA13</f>
         <v>0</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AA13:AA14" si="25">AB13</f>
         <v>0</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AB13:AB14" si="26">AC13</f>
         <v>0</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AC13:AC14" si="27">AD13</f>
         <v>0</v>
       </c>
       <c r="AD13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AD13:AD14" si="28">AE13</f>
         <v>0</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AE13:AE14" si="29">AF13</f>
         <v>0</v>
       </c>
       <c r="AF13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AF13:AF14" si="30">AG13</f>
         <v>0</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AG13:AG14" si="31">AH13</f>
         <v>0</v>
       </c>
       <c r="AH13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AH13:AH14" si="32">AI13</f>
         <v>0</v>
       </c>
       <c r="AI13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AI13:AI14" si="33">AJ13</f>
         <v>0</v>
       </c>
       <c r="AJ13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AJ13:AJ14" si="34">AK13</f>
         <v>0</v>
       </c>
       <c r="AK13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AK13:AK14" si="35">AL13</f>
         <v>0</v>
       </c>
       <c r="AL13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AL13:AL14" si="36">AM13</f>
         <v>0</v>
       </c>
       <c r="AM13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AM13:AM14" si="37">AN13</f>
         <v>0</v>
       </c>
     </row>
@@ -4977,156 +4528,118 @@
         <v>31</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
-        <v>1.0728312983511656E-4</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
-        <v>1.0728312983511656E-4</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>1.0728312983511656E-4</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
-        <v>1.0728312983511656E-4</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <f>'Technologies to power CCS'!B31</f>
-        <v>1.0728312983511656E-4</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <f>'Technologies to power CCS'!C31</f>
-        <v>1.481058739776992E-4</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <f>'Technologies to power CCS'!D31</f>
-        <v>1.861401877596074E-4</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <f>'Technologies to power CCS'!E31</f>
-        <v>2.2193262480603088E-4</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <f>'Technologies to power CCS'!F31</f>
-        <v>2.1525763325093273E-4</v>
+        <v>0</v>
       </c>
       <c r="K14">
-        <f>'Technologies to power CCS'!G31</f>
-        <v>2.1128641310043373E-4</v>
+        <v>0</v>
       </c>
       <c r="L14">
-        <f>'Technologies to power CCS'!H31</f>
-        <v>2.0855474895847758E-4</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <f>'Technologies to power CCS'!I31</f>
-        <v>2.0626790405407189E-4</v>
+        <v>0</v>
       </c>
       <c r="N14">
-        <f>'Technologies to power CCS'!J31</f>
-        <v>2.0314930173522008E-4</v>
+        <v>0</v>
       </c>
       <c r="O14">
-        <f>'Technologies to power CCS'!K31</f>
-        <v>1.9712870217559122E-4</v>
+        <v>0</v>
       </c>
       <c r="P14">
-        <f>'Technologies to power CCS'!L31</f>
-        <v>1.9224351255042548E-4</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <f>'Technologies to power CCS'!M31</f>
-        <v>1.88979901609504E-4</v>
+        <v>0</v>
       </c>
       <c r="R14">
-        <f>'Technologies to power CCS'!N31</f>
-        <v>1.8501228777610494E-4</v>
+        <v>0</v>
       </c>
       <c r="S14">
-        <f>'Technologies to power CCS'!O31</f>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="T14">
-        <f t="shared" si="3"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="U14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="V14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="W14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="X14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AF14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AH14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AI14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AJ14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AK14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AL14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AM14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert CCS files to same as master branch
</commit_message>
<xml_diff>
--- a/InputData/ccs/CPbE/CCS Percentages by Entity.xlsx
+++ b/InputData/ccs/CPbE/CCS Percentages by Entity.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-california\InputData\ccs\CPbE\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="18960" windowHeight="7163"/>
   </bookViews>
@@ -18,7 +13,7 @@
     <sheet name="CPbE-FoESCbES" sheetId="5" r:id="rId4"/>
     <sheet name="CPbE-PoICbI" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -241,7 +236,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
@@ -313,9 +308,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -363,7 +355,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -398,7 +390,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2515,7 +2507,7 @@
   <dimension ref="A1:AM3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2647,118 +2639,156 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="AB2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="AC2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="AE2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="AF2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="AG2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="AH2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="AI2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="AJ2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="AK2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="AL2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
       <c r="AM2">
-        <v>1</v>
+        <f>About!$I$24</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
@@ -2766,155 +2796,156 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <f>About!$I$23</f>
+        <v>1</v>
       </c>
       <c r="C3">
         <f>$B$3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:AM3" si="0">$B$3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2930,7 +2961,7 @@
   <dimension ref="A1:AM14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:AM14"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3062,117 +3093,155 @@
         <v>32</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <f t="shared" ref="B2:D14" si="0">C2</f>
+        <v>5.9005721409314106E-4</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.9005721409314106E-4</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.9005721409314106E-4</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <f>F2</f>
+        <v>5.9005721409314106E-4</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <f>'Technologies to power CCS'!B19</f>
+        <v>5.9005721409314106E-4</v>
       </c>
       <c r="G2">
+        <f>'Technologies to power CCS'!C19</f>
         <v>0</v>
       </c>
       <c r="H2">
+        <f>'Technologies to power CCS'!D19</f>
         <v>0</v>
       </c>
       <c r="I2">
+        <f>'Technologies to power CCS'!E19</f>
         <v>0</v>
       </c>
       <c r="J2">
+        <f>'Technologies to power CCS'!F19</f>
         <v>0</v>
       </c>
       <c r="K2">
+        <f>'Technologies to power CCS'!G19</f>
         <v>0</v>
       </c>
       <c r="L2">
+        <f>'Technologies to power CCS'!H19</f>
         <v>0</v>
       </c>
       <c r="M2">
+        <f>'Technologies to power CCS'!I19</f>
         <v>0</v>
       </c>
       <c r="N2">
+        <f>'Technologies to power CCS'!J19</f>
         <v>0</v>
       </c>
       <c r="O2">
+        <f>'Technologies to power CCS'!K19</f>
         <v>0</v>
       </c>
       <c r="P2">
+        <f>'Technologies to power CCS'!L19</f>
         <v>0</v>
       </c>
       <c r="Q2">
+        <f>'Technologies to power CCS'!M19</f>
         <v>0</v>
       </c>
       <c r="R2">
+        <f>'Technologies to power CCS'!N19</f>
         <v>0</v>
       </c>
       <c r="S2">
+        <f>'Technologies to power CCS'!O19</f>
         <v>0</v>
       </c>
       <c r="T2">
+        <f>S2</f>
         <v>0</v>
       </c>
       <c r="U2">
+        <f t="shared" ref="U2:AM14" si="1">T2</f>
         <v>0</v>
       </c>
       <c r="V2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3181,118 +3250,156 @@
         <v>26</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.3335464691512724</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.3335464691512724</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.3335464691512724</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <f t="shared" ref="E3:E14" si="2">F3</f>
+        <v>0.3335464691512724</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <f>'Technologies to power CCS'!B20</f>
+        <v>0.3335464691512724</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <f>'Technologies to power CCS'!C20</f>
+        <v>0.30616347531420662</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <f>'Technologies to power CCS'!D20</f>
+        <v>0.28003302126930857</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <f>'Technologies to power CCS'!E20</f>
+        <v>0.25791944378357839</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <f>'Technologies to power CCS'!F20</f>
+        <v>0.24105755214185653</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <f>'Technologies to power CCS'!G20</f>
+        <v>0.22761293681353043</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <f>'Technologies to power CCS'!H20</f>
+        <v>0.21576323530147837</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <f>'Technologies to power CCS'!I20</f>
+        <v>0.20459795910285011</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <f>'Technologies to power CCS'!J20</f>
+        <v>0.19296502094063003</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <f>'Technologies to power CCS'!K20</f>
+        <v>0.1865838936388145</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <f>'Technologies to power CCS'!L20</f>
+        <v>0.18044668164628119</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <f>'Technologies to power CCS'!M20</f>
+        <v>0.17592139040828728</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <f>'Technologies to power CCS'!N20</f>
+        <v>0.1707093578327098</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <f>'Technologies to power CCS'!O20</f>
+        <v>0.16286864789752623</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <f t="shared" ref="T3:AI14" si="3">S3</f>
+        <v>0.16286864789752623</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="AA3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="AB3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="AC3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="AD3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="AE3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="AF3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="AG3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="AH3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="AI3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="AJ3">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="AK3">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="AL3">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.16286864789752623</v>
       </c>
       <c r="AM3">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.16286864789752623</v>
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
@@ -3300,117 +3407,155 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.5672852969543393E-2</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.5672852969543393E-2</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.5672852969543393E-2</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>2.5672852969543393E-2</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <f>'Technologies to power CCS'!B21</f>
+        <v>2.5672852969543393E-2</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <f>'Technologies to power CCS'!C21</f>
+        <v>2.3627823761908948E-2</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <f>'Technologies to power CCS'!D21</f>
+        <v>2.2271673465437025E-2</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <f>'Technologies to power CCS'!E21</f>
+        <v>2.1243390846433275E-2</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <f>'Technologies to power CCS'!F21</f>
+        <v>2.0604460654779281E-2</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <f>'Technologies to power CCS'!G21</f>
+        <v>2.0224335461973515E-2</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <f>'Technologies to power CCS'!H21</f>
+        <v>1.9962860570305472E-2</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <f>'Technologies to power CCS'!I21</f>
+        <v>1.9743963776055761E-2</v>
       </c>
       <c r="N4">
+        <f>'Technologies to power CCS'!J21</f>
         <v>0</v>
       </c>
       <c r="O4">
+        <f>'Technologies to power CCS'!K21</f>
         <v>0</v>
       </c>
       <c r="P4">
+        <f>'Technologies to power CCS'!L21</f>
         <v>0</v>
       </c>
       <c r="Q4">
+        <f>'Technologies to power CCS'!M21</f>
         <v>0</v>
       </c>
       <c r="R4">
+        <f>'Technologies to power CCS'!N21</f>
         <v>0</v>
       </c>
       <c r="S4">
+        <f>'Technologies to power CCS'!O21</f>
         <v>0</v>
       </c>
       <c r="T4">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3419,118 +3564,156 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.15011055526529507</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.15011055526529507</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.15011055526529507</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.15011055526529507</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <f>'Technologies to power CCS'!B22</f>
+        <v>0.15011055526529507</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <f>'Technologies to power CCS'!C22</f>
+        <v>0.13815315924639782</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <f>'Technologies to power CCS'!D22</f>
+        <v>0.13022367535662133</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <f>'Technologies to power CCS'!E22</f>
+        <v>0.12421125145143937</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <f>'Technologies to power CCS'!F22</f>
+        <v>0.12047539217788203</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <f>'Technologies to power CCS'!G22</f>
+        <v>0.11825277968405075</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <f>'Technologies to power CCS'!H22</f>
+        <v>0.11672392189708072</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <f>'Technologies to power CCS'!I22</f>
+        <v>0.11544402054098295</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <f>'Technologies to power CCS'!J22</f>
+        <v>0.11369860119516798</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <f>'Technologies to power CCS'!K22</f>
+        <v>0.11032899203363489</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <f>'Technologies to power CCS'!L22</f>
+        <v>0.10759484910422214</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <f>'Technologies to power CCS'!M22</f>
+        <v>0.10576827133280721</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <f>'Technologies to power CCS'!N22</f>
+        <v>0.10354767722253042</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <f>'Technologies to power CCS'!O22</f>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="X5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="Y5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="AA5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="AB5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="AC5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="AD5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="AE5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="AF5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="AG5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="AH5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="AI5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="AJ5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="AK5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="AL5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
       <c r="AM5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9717680375187051E-2</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
@@ -3538,118 +3721,156 @@
         <v>33</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.0546961580838373E-2</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.0546961580838373E-2</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.0546961580838373E-2</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>9.0546961580838373E-2</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <f>'Technologies to power CCS'!B23</f>
+        <v>9.0546961580838373E-2</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <f>'Technologies to power CCS'!C23</f>
+        <v>0.10313105691313788</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <f>'Technologies to power CCS'!D23</f>
+        <v>0.11442968042521866</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <f>'Technologies to power CCS'!E23</f>
+        <v>0.12312822024238593</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <f>'Technologies to power CCS'!F23</f>
+        <v>0.12713115819800086</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <f>'Technologies to power CCS'!G23</f>
+        <v>0.12951857123056587</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <f>'Technologies to power CCS'!H23</f>
+        <v>0.13076382759696545</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <f>'Technologies to power CCS'!I23</f>
+        <v>0.13164017636730868</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <f>'Technologies to power CCS'!J23</f>
+        <v>0.14106687512493682</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <f>'Technologies to power CCS'!K23</f>
+        <v>0.14315486351991433</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <f>'Technologies to power CCS'!L23</f>
+        <v>0.14445177533038972</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <f>'Technologies to power CCS'!M23</f>
+        <v>0.14676179158994082</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <f>'Technologies to power CCS'!N23</f>
+        <v>0.15008196784397632</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <f>'Technologies to power CCS'!O23</f>
+        <v>0.15814289076082053</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="X6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="Y6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="Z6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="AA6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="AB6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="AC6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="AD6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="AE6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="AF6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="AG6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="AH6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="AI6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="AJ6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="AK6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="AL6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
       <c r="AM6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.15814289076082053</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
@@ -3657,118 +3878,156 @@
         <v>23</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.20936302787322997</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.20936302787322997</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.20936302787322997</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.20936302787322997</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <f>'Technologies to power CCS'!B24</f>
+        <v>0.20936302787322997</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <f>'Technologies to power CCS'!C24</f>
+        <v>0.253754730748458</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <f>'Technologies to power CCS'!D24</f>
+        <v>0.28778669079043501</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <f>'Technologies to power CCS'!E24</f>
+        <v>0.31689315630803538</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <f>'Technologies to power CCS'!F24</f>
+        <v>0.33883704050029317</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <f>'Technologies to power CCS'!G24</f>
+        <v>0.35529923226968935</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <f>'Technologies to power CCS'!H24</f>
+        <v>0.36962158157910979</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <f>'Technologies to power CCS'!I24</f>
+        <v>0.38302299639608717</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <f>'Technologies to power CCS'!J24</f>
+        <v>0.4089192294628245</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <f>'Technologies to power CCS'!K24</f>
+        <v>0.42083035340445213</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <f>'Technologies to power CCS'!L24</f>
+        <v>0.4318519817230248</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <f>'Technologies to power CCS'!M24</f>
+        <v>0.44571287754404737</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <f>'Technologies to power CCS'!N24</f>
+        <v>0.4598258397929757</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <f>'Technologies to power CCS'!O24</f>
+        <v>0.474699489310353</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="X7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="Y7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="Z7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="AA7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="AB7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="AC7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="AD7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="AE7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="AF7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="AG7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="AH7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="AI7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="AJ7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="AK7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="AL7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
       <c r="AM7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.474699489310353</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
@@ -3776,118 +4035,156 @@
         <v>24</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.3399662916406058E-2</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.3399662916406058E-2</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.3399662916406058E-2</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1.3399662916406058E-2</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <f>'Technologies to power CCS'!B25</f>
+        <v>1.3399662916406058E-2</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <f>'Technologies to power CCS'!C25</f>
+        <v>1.2332282439876422E-2</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <f>'Technologies to power CCS'!D25</f>
+        <v>1.1624454725587482E-2</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <f>'Technologies to power CCS'!E25</f>
+        <v>1.1087753935309303E-2</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <f>'Technologies to power CCS'!F25</f>
+        <v>1.0754271357216599E-2</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <f>'Technologies to power CCS'!G25</f>
+        <v>1.0555869198497669E-2</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <f>'Technologies to power CCS'!H25</f>
+        <v>1.0419395257965539E-2</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <f>'Technologies to power CCS'!I25</f>
+        <v>1.0305144486541431E-2</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <f>'Technologies to power CCS'!J25</f>
+        <v>1.0149339114691595E-2</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <f>'Technologies to power CCS'!K25</f>
+        <v>9.8485499606925375E-3</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <f>'Technologies to power CCS'!L25</f>
+        <v>9.6044858870192578E-3</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <f>'Technologies to power CCS'!M25</f>
+        <v>9.4414358844108204E-3</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <f>'Technologies to power CCS'!N25</f>
+        <v>9.2432138972942026E-3</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <f>'Technologies to power CCS'!O25</f>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="X8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="Y8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="Z8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="AA8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="AB8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="AC8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="AD8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="AE8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="AF8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="AG8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="AH8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="AI8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="AJ8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="AK8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="AL8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
       <c r="AM8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.901328100958306E-3</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
@@ -3895,118 +4192,156 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.4204286390169431E-2</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.4204286390169431E-2</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.4204286390169431E-2</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1.4204286390169431E-2</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <f>'Technologies to power CCS'!B26</f>
+        <v>1.4204286390169431E-2</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <f>'Technologies to power CCS'!C26</f>
+        <v>1.3072811809764917E-2</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <f>'Technologies to power CCS'!D26</f>
+        <v>1.2322480429686009E-2</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <f>'Technologies to power CCS'!E26</f>
+        <v>1.1753551809727395E-2</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <f>'Technologies to power CCS'!F26</f>
+        <v>1.1400044256969397E-2</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <f>'Technologies to power CCS'!G26</f>
+        <v>1.118972843779897E-2</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <f>'Technologies to power CCS'!H26</f>
+        <v>1.1045059504840972E-2</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <f>'Technologies to power CCS'!I26</f>
+        <v>1.0923948198703647E-2</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <f>'Technologies to power CCS'!J26</f>
+        <v>1.0758787019897256E-2</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <f>'Technologies to power CCS'!K26</f>
+        <v>1.043993606721931E-2</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <f>'Technologies to power CCS'!L26</f>
+        <v>1.0181216424670533E-2</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <f>'Technologies to power CCS'!M26</f>
+        <v>1.0008375589239333E-2</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <f>'Technologies to power CCS'!N26</f>
+        <v>9.7982507606225178E-3</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <f>'Technologies to power CCS'!O26</f>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="V9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="Y9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="Z9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="AA9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="AB9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="AC9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="AD9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="AE9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="AF9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="AG9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="AH9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="AI9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="AJ9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="AK9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="AL9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
       <c r="AM9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.4358353928493174E-3</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
@@ -4014,118 +4349,156 @@
         <v>27</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.9116641437250634E-2</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.9116641437250634E-2</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.9116641437250634E-2</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>2.9116641437250634E-2</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <f>'Technologies to power CCS'!B27</f>
+        <v>2.9116641437250634E-2</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <f>'Technologies to power CCS'!C27</f>
+        <v>2.6896026714350176E-2</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <f>'Technologies to power CCS'!D27</f>
+        <v>2.5445363666738333E-2</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <f>'Technologies to power CCS'!E27</f>
+        <v>2.4359324898709948E-2</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <f>'Technologies to power CCS'!F27</f>
+        <v>2.3626677825622375E-2</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <f>'Technologies to power CCS'!G27</f>
+        <v>2.3190796701903604E-2</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <f>'Technologies to power CCS'!H27</f>
+        <v>2.2890969245682499E-2</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <f>'Technologies to power CCS'!I27</f>
+        <v>2.2639965148974931E-2</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <f>'Technologies to power CCS'!J27</f>
+        <v>2.2297667358457757E-2</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <f>'Technologies to power CCS'!K27</f>
+        <v>2.1636846350792893E-2</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <f>'Technologies to power CCS'!L27</f>
+        <v>2.1100647937534699E-2</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <f>'Technologies to power CCS'!M27</f>
+        <v>2.0742434000659161E-2</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <f>'Technologies to power CCS'!N27</f>
+        <v>2.0306948706305276E-2</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <f>'Technologies to power CCS'!O27</f>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="W10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="X10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="Y10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="Z10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="AA10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="AB10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="AC10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="AD10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="AE10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="AF10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="AG10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="AH10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="AI10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="AJ10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="AK10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="AL10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
       <c r="AM10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.9627107758237932E-2</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
@@ -4133,118 +4506,156 @@
         <v>28</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.8085511091466378E-3</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.8085511091466378E-3</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.8085511091466378E-3</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>3.8085511091466378E-3</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <f>'Technologies to power CCS'!B28</f>
+        <v>3.8085511091466378E-3</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <f>'Technologies to power CCS'!C28</f>
+        <v>3.5051723508055482E-3</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <f>'Technologies to power CCS'!D28</f>
+        <v>3.3039883327330316E-3</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <f>'Technologies to power CCS'!E28</f>
+        <v>3.1514432722456387E-3</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <f>'Technologies to power CCS'!F28</f>
+        <v>3.0566583921632444E-3</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <f>'Technologies to power CCS'!G28</f>
+        <v>3.000267066026159E-3</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <f>'Technologies to power CCS'!H28</f>
+        <v>2.9614774352103817E-3</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <f>'Technologies to power CCS'!I28</f>
+        <v>2.9290042375678207E-3</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <f>'Technologies to power CCS'!J28</f>
+        <v>2.8847200846401251E-3</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <f>'Technologies to power CCS'!K28</f>
+        <v>2.7992275708933951E-3</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <f>'Technologies to power CCS'!L28</f>
+        <v>2.729857878216042E-3</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <f>'Technologies to power CCS'!M28</f>
+        <v>2.6835146028549571E-3</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <f>'Technologies to power CCS'!N28</f>
+        <v>2.6271744864206901E-3</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <f>'Technologies to power CCS'!O28</f>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="V11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="W11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="X11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="Y11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="Z11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="AA11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="AB11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="AC11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="AD11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="AE11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="AF11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="AG11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="AH11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="AI11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="AJ11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="AK11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="AL11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
       <c r="AM11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5300011816174529E-3</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
@@ -4252,118 +4663,156 @@
         <v>29</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.12953365096291972</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.12953365096291972</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.12953365096291972</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0.12953365096291972</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <f>'Technologies to power CCS'!B29</f>
+        <v>0.12953365096291972</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <f>'Technologies to power CCS'!C29</f>
+        <v>0.11921535482711602</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <f>'Technologies to power CCS'!D29</f>
+        <v>0.11237283135047499</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <f>'Technologies to power CCS'!E29</f>
+        <v>0.10603053082732931</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <f>'Technologies to power CCS'!F29</f>
+        <v>0.10284148686196562</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <f>'Technologies to power CCS'!G29</f>
+        <v>0.10094419672286321</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <f>'Technologies to power CCS'!H29</f>
+        <v>9.9639116862402247E-2</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <f>'Technologies to power CCS'!I29</f>
+        <v>9.854655384087338E-2</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <f>'Technologies to power CCS'!J29</f>
+        <v>9.7056610397018739E-2</v>
       </c>
       <c r="O12">
-        <v>1</v>
+        <f>'Technologies to power CCS'!K29</f>
+        <v>9.4180208751410463E-2</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <f>'Technologies to power CCS'!L29</f>
+        <v>9.1846260556091283E-2</v>
       </c>
       <c r="Q12">
-        <v>1</v>
+        <f>'Technologies to power CCS'!M29</f>
+        <v>8.2770929146143452E-2</v>
       </c>
       <c r="R12">
-        <v>1</v>
+        <f>'Technologies to power CCS'!N29</f>
+        <v>7.3674557169388963E-2</v>
       </c>
       <c r="S12">
-        <v>1</v>
+        <f>'Technologies to power CCS'!O29</f>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="T12">
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="U12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="V12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="W12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="X12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="Y12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="Z12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="AA12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="AB12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="AC12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="AD12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="AE12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="AF12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="AG12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="AH12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="AI12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="AJ12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="AK12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="AL12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
       <c r="AM12">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6.3863216305693693E-2</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
@@ -4371,155 +4820,155 @@
         <v>30</v>
       </c>
       <c r="B13">
-        <f t="shared" ref="B2:D14" si="0">C13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:C14" si="1">D13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D13">
-        <f t="shared" ref="D13:D14" si="2">E13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E13">
-        <f t="shared" ref="E13:E14" si="3">F13</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:F14" si="4">G13</f>
+        <f>'Technologies to power CCS'!B30</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13:G14" si="5">H13</f>
+        <f>'Technologies to power CCS'!C30</f>
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" ref="H13:H14" si="6">I13</f>
+        <f>'Technologies to power CCS'!D30</f>
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" ref="I13:I14" si="7">J13</f>
+        <f>'Technologies to power CCS'!E30</f>
         <v>0</v>
       </c>
       <c r="J13">
-        <f t="shared" ref="J13:J14" si="8">K13</f>
+        <f>'Technologies to power CCS'!F30</f>
         <v>0</v>
       </c>
       <c r="K13">
-        <f t="shared" ref="K13:K14" si="9">L13</f>
+        <f>'Technologies to power CCS'!G30</f>
         <v>0</v>
       </c>
       <c r="L13">
-        <f t="shared" ref="L13:L14" si="10">M13</f>
+        <f>'Technologies to power CCS'!H30</f>
         <v>0</v>
       </c>
       <c r="M13">
-        <f t="shared" ref="M13:M14" si="11">N13</f>
+        <f>'Technologies to power CCS'!I30</f>
         <v>0</v>
       </c>
       <c r="N13">
-        <f t="shared" ref="N13:N14" si="12">O13</f>
+        <f>'Technologies to power CCS'!J30</f>
         <v>0</v>
       </c>
       <c r="O13">
-        <f t="shared" ref="O13:O14" si="13">P13</f>
+        <f>'Technologies to power CCS'!K30</f>
         <v>0</v>
       </c>
       <c r="P13">
-        <f t="shared" ref="P13:P14" si="14">Q13</f>
+        <f>'Technologies to power CCS'!L30</f>
         <v>0</v>
       </c>
       <c r="Q13">
-        <f t="shared" ref="Q13:Q14" si="15">R13</f>
+        <f>'Technologies to power CCS'!M30</f>
         <v>0</v>
       </c>
       <c r="R13">
-        <f t="shared" ref="R13:R14" si="16">S13</f>
+        <f>'Technologies to power CCS'!N30</f>
         <v>0</v>
       </c>
       <c r="S13">
-        <f t="shared" ref="S13:S14" si="17">T13</f>
+        <f>'Technologies to power CCS'!O30</f>
         <v>0</v>
       </c>
       <c r="T13">
-        <f t="shared" ref="T13:T14" si="18">U13</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U13">
-        <f t="shared" ref="U13:U14" si="19">V13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V13">
-        <f t="shared" ref="V13:V14" si="20">W13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W13">
-        <f t="shared" ref="W13:W14" si="21">X13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X13">
-        <f t="shared" ref="X13:X14" si="22">Y13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y13">
-        <f t="shared" ref="Y13:Y14" si="23">Z13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z13">
-        <f t="shared" ref="Z13:Z14" si="24">AA13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA13">
-        <f t="shared" ref="AA13:AA14" si="25">AB13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB13">
-        <f t="shared" ref="AB13:AB14" si="26">AC13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC13">
-        <f t="shared" ref="AC13:AC14" si="27">AD13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD13">
-        <f t="shared" ref="AD13:AD14" si="28">AE13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE13">
-        <f t="shared" ref="AE13:AE14" si="29">AF13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF13">
-        <f t="shared" ref="AF13:AF14" si="30">AG13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG13">
-        <f t="shared" ref="AG13:AG14" si="31">AH13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH13">
-        <f t="shared" ref="AH13:AH14" si="32">AI13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI13">
-        <f t="shared" ref="AI13:AI14" si="33">AJ13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ13">
-        <f t="shared" ref="AJ13:AJ14" si="34">AK13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK13">
-        <f t="shared" ref="AK13:AK14" si="35">AL13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL13">
-        <f t="shared" ref="AL13:AL14" si="36">AM13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM13">
-        <f t="shared" ref="AM13:AM14" si="37">AN13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4528,118 +4977,156 @@
         <v>31</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.0728312983511656E-4</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.0728312983511656E-4</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.0728312983511656E-4</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1.0728312983511656E-4</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <f>'Technologies to power CCS'!B31</f>
+        <v>1.0728312983511656E-4</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <f>'Technologies to power CCS'!C31</f>
+        <v>1.481058739776992E-4</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <f>'Technologies to power CCS'!D31</f>
+        <v>1.861401877596074E-4</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <f>'Technologies to power CCS'!E31</f>
+        <v>2.2193262480603088E-4</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <f>'Technologies to power CCS'!F31</f>
+        <v>2.1525763325093273E-4</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <f>'Technologies to power CCS'!G31</f>
+        <v>2.1128641310043373E-4</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <f>'Technologies to power CCS'!H31</f>
+        <v>2.0855474895847758E-4</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <f>'Technologies to power CCS'!I31</f>
+        <v>2.0626790405407189E-4</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <f>'Technologies to power CCS'!J31</f>
+        <v>2.0314930173522008E-4</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <f>'Technologies to power CCS'!K31</f>
+        <v>1.9712870217559122E-4</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <f>'Technologies to power CCS'!L31</f>
+        <v>1.9224351255042548E-4</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <f>'Technologies to power CCS'!M31</f>
+        <v>1.88979901609504E-4</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <f>'Technologies to power CCS'!N31</f>
+        <v>1.8501228777610494E-4</v>
       </c>
       <c r="S14">
-        <v>0</v>
+        <f>'Technologies to power CCS'!O31</f>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="V14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="W14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="X14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="Y14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="Z14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="AA14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="AB14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="AC14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="AD14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="AE14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="AF14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="AG14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="AH14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="AI14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="AJ14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="AK14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="AL14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
       <c r="AM14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1380291675640448E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert CCS files to same as master branch"
This reverts commit f4907dc47792ea2602c07a79adaf3b0bf6c0e918.
</commit_message>
<xml_diff>
--- a/InputData/ccs/CPbE/CCS Percentages by Entity.xlsx
+++ b/InputData/ccs/CPbE/CCS Percentages by Entity.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-california\InputData\ccs\CPbE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="18960" windowHeight="7163"/>
   </bookViews>
@@ -13,7 +18,7 @@
     <sheet name="CPbE-FoESCbES" sheetId="5" r:id="rId4"/>
     <sheet name="CPbE-PoICbI" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -236,7 +241,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
@@ -308,6 +313,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -355,7 +363,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,7 +398,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2507,7 +2515,7 @@
   <dimension ref="A1:AM3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2639,156 +2647,118 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM2">
-        <f>About!$I$24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
@@ -2796,156 +2766,155 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <f>About!$I$23</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <f>$B$3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:AM3" si="0">$B$3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2961,7 +2930,7 @@
   <dimension ref="A1:AM14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B14" sqref="B14:AM14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3093,155 +3062,117 @@
         <v>32</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:D14" si="0">C2</f>
-        <v>5.9005721409314106E-4</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <f t="shared" si="0"/>
-        <v>5.9005721409314106E-4</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <f t="shared" si="0"/>
-        <v>5.9005721409314106E-4</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <f>F2</f>
-        <v>5.9005721409314106E-4</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <f>'Technologies to power CCS'!B19</f>
-        <v>5.9005721409314106E-4</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <f>'Technologies to power CCS'!C19</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f>'Technologies to power CCS'!D19</f>
         <v>0</v>
       </c>
       <c r="I2">
-        <f>'Technologies to power CCS'!E19</f>
         <v>0</v>
       </c>
       <c r="J2">
-        <f>'Technologies to power CCS'!F19</f>
         <v>0</v>
       </c>
       <c r="K2">
-        <f>'Technologies to power CCS'!G19</f>
         <v>0</v>
       </c>
       <c r="L2">
-        <f>'Technologies to power CCS'!H19</f>
         <v>0</v>
       </c>
       <c r="M2">
-        <f>'Technologies to power CCS'!I19</f>
         <v>0</v>
       </c>
       <c r="N2">
-        <f>'Technologies to power CCS'!J19</f>
         <v>0</v>
       </c>
       <c r="O2">
-        <f>'Technologies to power CCS'!K19</f>
         <v>0</v>
       </c>
       <c r="P2">
-        <f>'Technologies to power CCS'!L19</f>
         <v>0</v>
       </c>
       <c r="Q2">
-        <f>'Technologies to power CCS'!M19</f>
         <v>0</v>
       </c>
       <c r="R2">
-        <f>'Technologies to power CCS'!N19</f>
         <v>0</v>
       </c>
       <c r="S2">
-        <f>'Technologies to power CCS'!O19</f>
         <v>0</v>
       </c>
       <c r="T2">
-        <f>S2</f>
         <v>0</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:AM14" si="1">T2</f>
         <v>0</v>
       </c>
       <c r="V2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3250,156 +3181,118 @@
         <v>26</v>
       </c>
       <c r="B3">
-        <f t="shared" si="0"/>
-        <v>0.3335464691512724</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
-        <v>0.3335464691512724</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
-        <v>0.3335464691512724</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E14" si="2">F3</f>
-        <v>0.3335464691512724</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <f>'Technologies to power CCS'!B20</f>
-        <v>0.3335464691512724</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <f>'Technologies to power CCS'!C20</f>
-        <v>0.30616347531420662</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <f>'Technologies to power CCS'!D20</f>
-        <v>0.28003302126930857</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <f>'Technologies to power CCS'!E20</f>
-        <v>0.25791944378357839</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <f>'Technologies to power CCS'!F20</f>
-        <v>0.24105755214185653</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <f>'Technologies to power CCS'!G20</f>
-        <v>0.22761293681353043</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <f>'Technologies to power CCS'!H20</f>
-        <v>0.21576323530147837</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <f>'Technologies to power CCS'!I20</f>
-        <v>0.20459795910285011</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <f>'Technologies to power CCS'!J20</f>
-        <v>0.19296502094063003</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <f>'Technologies to power CCS'!K20</f>
-        <v>0.1865838936388145</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <f>'Technologies to power CCS'!L20</f>
-        <v>0.18044668164628119</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <f>'Technologies to power CCS'!M20</f>
-        <v>0.17592139040828728</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <f>'Technologies to power CCS'!N20</f>
-        <v>0.1707093578327098</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <f>'Technologies to power CCS'!O20</f>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:AI14" si="3">S3</f>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="U3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="Y3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="Z3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AA3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AB3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AC3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AD3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AE3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AF3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AG3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AH3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AI3">
-        <f t="shared" si="3"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AJ3">
-        <f t="shared" si="1"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AK3">
-        <f t="shared" si="1"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AL3">
-        <f t="shared" si="1"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
       <c r="AM3">
-        <f t="shared" si="1"/>
-        <v>0.16286864789752623</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
@@ -3407,155 +3300,117 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>2.5672852969543393E-2</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>2.5672852969543393E-2</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>2.5672852969543393E-2</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="2"/>
-        <v>2.5672852969543393E-2</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <f>'Technologies to power CCS'!B21</f>
-        <v>2.5672852969543393E-2</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <f>'Technologies to power CCS'!C21</f>
-        <v>2.3627823761908948E-2</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <f>'Technologies to power CCS'!D21</f>
-        <v>2.2271673465437025E-2</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <f>'Technologies to power CCS'!E21</f>
-        <v>2.1243390846433275E-2</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <f>'Technologies to power CCS'!F21</f>
-        <v>2.0604460654779281E-2</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <f>'Technologies to power CCS'!G21</f>
-        <v>2.0224335461973515E-2</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <f>'Technologies to power CCS'!H21</f>
-        <v>1.9962860570305472E-2</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <f>'Technologies to power CCS'!I21</f>
-        <v>1.9743963776055761E-2</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <f>'Technologies to power CCS'!J21</f>
         <v>0</v>
       </c>
       <c r="O4">
-        <f>'Technologies to power CCS'!K21</f>
         <v>0</v>
       </c>
       <c r="P4">
-        <f>'Technologies to power CCS'!L21</f>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f>'Technologies to power CCS'!M21</f>
         <v>0</v>
       </c>
       <c r="R4">
-        <f>'Technologies to power CCS'!N21</f>
         <v>0</v>
       </c>
       <c r="S4">
-        <f>'Technologies to power CCS'!O21</f>
         <v>0</v>
       </c>
       <c r="T4">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3564,156 +3419,118 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>0.15011055526529507</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>0.15011055526529507</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0.15011055526529507</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
-        <v>0.15011055526529507</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <f>'Technologies to power CCS'!B22</f>
-        <v>0.15011055526529507</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <f>'Technologies to power CCS'!C22</f>
-        <v>0.13815315924639782</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <f>'Technologies to power CCS'!D22</f>
-        <v>0.13022367535662133</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <f>'Technologies to power CCS'!E22</f>
-        <v>0.12421125145143937</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <f>'Technologies to power CCS'!F22</f>
-        <v>0.12047539217788203</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <f>'Technologies to power CCS'!G22</f>
-        <v>0.11825277968405075</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <f>'Technologies to power CCS'!H22</f>
-        <v>0.11672392189708072</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <f>'Technologies to power CCS'!I22</f>
-        <v>0.11544402054098295</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <f>'Technologies to power CCS'!J22</f>
-        <v>0.11369860119516798</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <f>'Technologies to power CCS'!K22</f>
-        <v>0.11032899203363489</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <f>'Technologies to power CCS'!L22</f>
-        <v>0.10759484910422214</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <f>'Technologies to power CCS'!M22</f>
-        <v>0.10576827133280721</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <f>'Technologies to power CCS'!N22</f>
-        <v>0.10354767722253042</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <f>'Technologies to power CCS'!O22</f>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <f t="shared" si="3"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="U5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="V5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="W5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="X5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="Z5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AA5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AB5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AC5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AD5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AE5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AF5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AG5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AH5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AI5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AJ5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AK5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AL5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
       <c r="AM5">
-        <f t="shared" si="1"/>
-        <v>9.9717680375187051E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
@@ -3721,156 +3538,118 @@
         <v>33</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>9.0546961580838373E-2</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>9.0546961580838373E-2</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>9.0546961580838373E-2</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
-        <v>9.0546961580838373E-2</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <f>'Technologies to power CCS'!B23</f>
-        <v>9.0546961580838373E-2</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <f>'Technologies to power CCS'!C23</f>
-        <v>0.10313105691313788</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <f>'Technologies to power CCS'!D23</f>
-        <v>0.11442968042521866</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <f>'Technologies to power CCS'!E23</f>
-        <v>0.12312822024238593</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <f>'Technologies to power CCS'!F23</f>
-        <v>0.12713115819800086</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <f>'Technologies to power CCS'!G23</f>
-        <v>0.12951857123056587</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <f>'Technologies to power CCS'!H23</f>
-        <v>0.13076382759696545</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <f>'Technologies to power CCS'!I23</f>
-        <v>0.13164017636730868</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <f>'Technologies to power CCS'!J23</f>
-        <v>0.14106687512493682</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <f>'Technologies to power CCS'!K23</f>
-        <v>0.14315486351991433</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <f>'Technologies to power CCS'!L23</f>
-        <v>0.14445177533038972</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <f>'Technologies to power CCS'!M23</f>
-        <v>0.14676179158994082</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <f>'Technologies to power CCS'!N23</f>
-        <v>0.15008196784397632</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <f>'Technologies to power CCS'!O23</f>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <f t="shared" si="3"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="U6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="X6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="Z6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AA6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AC6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AD6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AE6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AF6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AG6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AH6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AI6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AJ6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AK6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AL6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
       <c r="AM6">
-        <f t="shared" si="1"/>
-        <v>0.15814289076082053</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
@@ -3878,156 +3657,118 @@
         <v>23</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>0.20936302787322997</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>0.20936302787322997</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>0.20936302787322997</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
-        <v>0.20936302787322997</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <f>'Technologies to power CCS'!B24</f>
-        <v>0.20936302787322997</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <f>'Technologies to power CCS'!C24</f>
-        <v>0.253754730748458</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <f>'Technologies to power CCS'!D24</f>
-        <v>0.28778669079043501</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <f>'Technologies to power CCS'!E24</f>
-        <v>0.31689315630803538</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <f>'Technologies to power CCS'!F24</f>
-        <v>0.33883704050029317</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <f>'Technologies to power CCS'!G24</f>
-        <v>0.35529923226968935</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <f>'Technologies to power CCS'!H24</f>
-        <v>0.36962158157910979</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <f>'Technologies to power CCS'!I24</f>
-        <v>0.38302299639608717</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <f>'Technologies to power CCS'!J24</f>
-        <v>0.4089192294628245</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <f>'Technologies to power CCS'!K24</f>
-        <v>0.42083035340445213</v>
+        <v>0</v>
       </c>
       <c r="P7">
-        <f>'Technologies to power CCS'!L24</f>
-        <v>0.4318519817230248</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <f>'Technologies to power CCS'!M24</f>
-        <v>0.44571287754404737</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <f>'Technologies to power CCS'!N24</f>
-        <v>0.4598258397929757</v>
+        <v>0</v>
       </c>
       <c r="S7">
-        <f>'Technologies to power CCS'!O24</f>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="T7">
-        <f t="shared" si="3"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="U7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="V7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="W7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="X7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AD7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AE7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AF7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AG7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AH7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AI7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AJ7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AK7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AL7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
       <c r="AM7">
-        <f t="shared" si="1"/>
-        <v>0.474699489310353</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
@@ -4035,156 +3776,118 @@
         <v>24</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>1.3399662916406058E-2</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>1.3399662916406058E-2</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1.3399662916406058E-2</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
-        <v>1.3399662916406058E-2</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <f>'Technologies to power CCS'!B25</f>
-        <v>1.3399662916406058E-2</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <f>'Technologies to power CCS'!C25</f>
-        <v>1.2332282439876422E-2</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <f>'Technologies to power CCS'!D25</f>
-        <v>1.1624454725587482E-2</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <f>'Technologies to power CCS'!E25</f>
-        <v>1.1087753935309303E-2</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <f>'Technologies to power CCS'!F25</f>
-        <v>1.0754271357216599E-2</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <f>'Technologies to power CCS'!G25</f>
-        <v>1.0555869198497669E-2</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <f>'Technologies to power CCS'!H25</f>
-        <v>1.0419395257965539E-2</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <f>'Technologies to power CCS'!I25</f>
-        <v>1.0305144486541431E-2</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <f>'Technologies to power CCS'!J25</f>
-        <v>1.0149339114691595E-2</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <f>'Technologies to power CCS'!K25</f>
-        <v>9.8485499606925375E-3</v>
+        <v>0</v>
       </c>
       <c r="P8">
-        <f>'Technologies to power CCS'!L25</f>
-        <v>9.6044858870192578E-3</v>
+        <v>0</v>
       </c>
       <c r="Q8">
-        <f>'Technologies to power CCS'!M25</f>
-        <v>9.4414358844108204E-3</v>
+        <v>0</v>
       </c>
       <c r="R8">
-        <f>'Technologies to power CCS'!N25</f>
-        <v>9.2432138972942026E-3</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <f>'Technologies to power CCS'!O25</f>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="T8">
-        <f t="shared" si="3"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="U8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="V8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="W8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="X8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AA8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AB8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AD8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AE8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AF8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AG8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AH8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AI8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AJ8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AK8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AL8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
       <c r="AM8">
-        <f t="shared" si="1"/>
-        <v>8.901328100958306E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
@@ -4192,156 +3895,118 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>1.4204286390169431E-2</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>1.4204286390169431E-2</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>1.4204286390169431E-2</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
-        <v>1.4204286390169431E-2</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <f>'Technologies to power CCS'!B26</f>
-        <v>1.4204286390169431E-2</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <f>'Technologies to power CCS'!C26</f>
-        <v>1.3072811809764917E-2</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <f>'Technologies to power CCS'!D26</f>
-        <v>1.2322480429686009E-2</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <f>'Technologies to power CCS'!E26</f>
-        <v>1.1753551809727395E-2</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <f>'Technologies to power CCS'!F26</f>
-        <v>1.1400044256969397E-2</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <f>'Technologies to power CCS'!G26</f>
-        <v>1.118972843779897E-2</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <f>'Technologies to power CCS'!H26</f>
-        <v>1.1045059504840972E-2</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <f>'Technologies to power CCS'!I26</f>
-        <v>1.0923948198703647E-2</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <f>'Technologies to power CCS'!J26</f>
-        <v>1.0758787019897256E-2</v>
+        <v>0</v>
       </c>
       <c r="O9">
-        <f>'Technologies to power CCS'!K26</f>
-        <v>1.043993606721931E-2</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <f>'Technologies to power CCS'!L26</f>
-        <v>1.0181216424670533E-2</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <f>'Technologies to power CCS'!M26</f>
-        <v>1.0008375589239333E-2</v>
+        <v>0</v>
       </c>
       <c r="R9">
-        <f>'Technologies to power CCS'!N26</f>
-        <v>9.7982507606225178E-3</v>
+        <v>0</v>
       </c>
       <c r="S9">
-        <f>'Technologies to power CCS'!O26</f>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="T9">
-        <f t="shared" si="3"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="U9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="V9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="W9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AB9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AD9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AE9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AF9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AG9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AH9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AI9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AJ9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AK9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AL9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
       <c r="AM9">
-        <f t="shared" si="1"/>
-        <v>9.4358353928493174E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
@@ -4349,156 +4014,118 @@
         <v>27</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>2.9116641437250634E-2</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>2.9116641437250634E-2</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>2.9116641437250634E-2</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
-        <v>2.9116641437250634E-2</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <f>'Technologies to power CCS'!B27</f>
-        <v>2.9116641437250634E-2</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <f>'Technologies to power CCS'!C27</f>
-        <v>2.6896026714350176E-2</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <f>'Technologies to power CCS'!D27</f>
-        <v>2.5445363666738333E-2</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <f>'Technologies to power CCS'!E27</f>
-        <v>2.4359324898709948E-2</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <f>'Technologies to power CCS'!F27</f>
-        <v>2.3626677825622375E-2</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <f>'Technologies to power CCS'!G27</f>
-        <v>2.3190796701903604E-2</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <f>'Technologies to power CCS'!H27</f>
-        <v>2.2890969245682499E-2</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <f>'Technologies to power CCS'!I27</f>
-        <v>2.2639965148974931E-2</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <f>'Technologies to power CCS'!J27</f>
-        <v>2.2297667358457757E-2</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <f>'Technologies to power CCS'!K27</f>
-        <v>2.1636846350792893E-2</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <f>'Technologies to power CCS'!L27</f>
-        <v>2.1100647937534699E-2</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <f>'Technologies to power CCS'!M27</f>
-        <v>2.0742434000659161E-2</v>
+        <v>0</v>
       </c>
       <c r="R10">
-        <f>'Technologies to power CCS'!N27</f>
-        <v>2.0306948706305276E-2</v>
+        <v>0</v>
       </c>
       <c r="S10">
-        <f>'Technologies to power CCS'!O27</f>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="T10">
-        <f t="shared" si="3"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="U10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="V10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="W10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="X10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AB10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AD10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AE10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AF10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AH10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AI10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AJ10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AK10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AL10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
       <c r="AM10">
-        <f t="shared" si="1"/>
-        <v>1.9627107758237932E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
@@ -4506,156 +4133,118 @@
         <v>28</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
-        <v>3.8085511091466378E-3</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>3.8085511091466378E-3</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>3.8085511091466378E-3</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
-        <v>3.8085511091466378E-3</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <f>'Technologies to power CCS'!B28</f>
-        <v>3.8085511091466378E-3</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <f>'Technologies to power CCS'!C28</f>
-        <v>3.5051723508055482E-3</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <f>'Technologies to power CCS'!D28</f>
-        <v>3.3039883327330316E-3</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <f>'Technologies to power CCS'!E28</f>
-        <v>3.1514432722456387E-3</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <f>'Technologies to power CCS'!F28</f>
-        <v>3.0566583921632444E-3</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <f>'Technologies to power CCS'!G28</f>
-        <v>3.000267066026159E-3</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <f>'Technologies to power CCS'!H28</f>
-        <v>2.9614774352103817E-3</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <f>'Technologies to power CCS'!I28</f>
-        <v>2.9290042375678207E-3</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <f>'Technologies to power CCS'!J28</f>
-        <v>2.8847200846401251E-3</v>
+        <v>0</v>
       </c>
       <c r="O11">
-        <f>'Technologies to power CCS'!K28</f>
-        <v>2.7992275708933951E-3</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <f>'Technologies to power CCS'!L28</f>
-        <v>2.729857878216042E-3</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <f>'Technologies to power CCS'!M28</f>
-        <v>2.6835146028549571E-3</v>
+        <v>0</v>
       </c>
       <c r="R11">
-        <f>'Technologies to power CCS'!N28</f>
-        <v>2.6271744864206901E-3</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <f>'Technologies to power CCS'!O28</f>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="T11">
-        <f t="shared" si="3"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="U11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="V11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="W11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="X11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AD11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AE11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AF11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AH11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AI11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AJ11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AK11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AL11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
       <c r="AM11">
-        <f t="shared" si="1"/>
-        <v>2.5300011816174529E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
@@ -4663,156 +4252,118 @@
         <v>29</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
-        <v>0.12953365096291972</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>0.12953365096291972</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0.12953365096291972</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
-        <v>0.12953365096291972</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <f>'Technologies to power CCS'!B29</f>
-        <v>0.12953365096291972</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <f>'Technologies to power CCS'!C29</f>
-        <v>0.11921535482711602</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <f>'Technologies to power CCS'!D29</f>
-        <v>0.11237283135047499</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <f>'Technologies to power CCS'!E29</f>
-        <v>0.10603053082732931</v>
+        <v>1</v>
       </c>
       <c r="J12">
-        <f>'Technologies to power CCS'!F29</f>
-        <v>0.10284148686196562</v>
+        <v>1</v>
       </c>
       <c r="K12">
-        <f>'Technologies to power CCS'!G29</f>
-        <v>0.10094419672286321</v>
+        <v>1</v>
       </c>
       <c r="L12">
-        <f>'Technologies to power CCS'!H29</f>
-        <v>9.9639116862402247E-2</v>
+        <v>1</v>
       </c>
       <c r="M12">
-        <f>'Technologies to power CCS'!I29</f>
-        <v>9.854655384087338E-2</v>
+        <v>1</v>
       </c>
       <c r="N12">
-        <f>'Technologies to power CCS'!J29</f>
-        <v>9.7056610397018739E-2</v>
+        <v>1</v>
       </c>
       <c r="O12">
-        <f>'Technologies to power CCS'!K29</f>
-        <v>9.4180208751410463E-2</v>
+        <v>1</v>
       </c>
       <c r="P12">
-        <f>'Technologies to power CCS'!L29</f>
-        <v>9.1846260556091283E-2</v>
+        <v>1</v>
       </c>
       <c r="Q12">
-        <f>'Technologies to power CCS'!M29</f>
-        <v>8.2770929146143452E-2</v>
+        <v>1</v>
       </c>
       <c r="R12">
-        <f>'Technologies to power CCS'!N29</f>
-        <v>7.3674557169388963E-2</v>
+        <v>1</v>
       </c>
       <c r="S12">
-        <f>'Technologies to power CCS'!O29</f>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="T12">
-        <f t="shared" si="3"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="U12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="V12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="W12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="X12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AB12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AD12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AE12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AF12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AG12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AH12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AI12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AJ12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AK12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AL12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
       <c r="AM12">
-        <f t="shared" si="1"/>
-        <v>6.3863216305693693E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
@@ -4820,155 +4371,155 @@
         <v>30</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B2:D14" si="0">C13</f>
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C13:C14" si="1">D13</f>
         <v>0</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D13:D14" si="2">E13</f>
         <v>0</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E13:E14" si="3">F13</f>
         <v>0</v>
       </c>
       <c r="F13">
-        <f>'Technologies to power CCS'!B30</f>
+        <f t="shared" ref="F13:F14" si="4">G13</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <f>'Technologies to power CCS'!C30</f>
+        <f t="shared" ref="G13:G14" si="5">H13</f>
         <v>0</v>
       </c>
       <c r="H13">
-        <f>'Technologies to power CCS'!D30</f>
+        <f t="shared" ref="H13:H14" si="6">I13</f>
         <v>0</v>
       </c>
       <c r="I13">
-        <f>'Technologies to power CCS'!E30</f>
+        <f t="shared" ref="I13:I14" si="7">J13</f>
         <v>0</v>
       </c>
       <c r="J13">
-        <f>'Technologies to power CCS'!F30</f>
+        <f t="shared" ref="J13:J14" si="8">K13</f>
         <v>0</v>
       </c>
       <c r="K13">
-        <f>'Technologies to power CCS'!G30</f>
+        <f t="shared" ref="K13:K14" si="9">L13</f>
         <v>0</v>
       </c>
       <c r="L13">
-        <f>'Technologies to power CCS'!H30</f>
+        <f t="shared" ref="L13:L14" si="10">M13</f>
         <v>0</v>
       </c>
       <c r="M13">
-        <f>'Technologies to power CCS'!I30</f>
+        <f t="shared" ref="M13:M14" si="11">N13</f>
         <v>0</v>
       </c>
       <c r="N13">
-        <f>'Technologies to power CCS'!J30</f>
+        <f t="shared" ref="N13:N14" si="12">O13</f>
         <v>0</v>
       </c>
       <c r="O13">
-        <f>'Technologies to power CCS'!K30</f>
+        <f t="shared" ref="O13:O14" si="13">P13</f>
         <v>0</v>
       </c>
       <c r="P13">
-        <f>'Technologies to power CCS'!L30</f>
+        <f t="shared" ref="P13:P14" si="14">Q13</f>
         <v>0</v>
       </c>
       <c r="Q13">
-        <f>'Technologies to power CCS'!M30</f>
+        <f t="shared" ref="Q13:Q14" si="15">R13</f>
         <v>0</v>
       </c>
       <c r="R13">
-        <f>'Technologies to power CCS'!N30</f>
+        <f t="shared" ref="R13:R14" si="16">S13</f>
         <v>0</v>
       </c>
       <c r="S13">
-        <f>'Technologies to power CCS'!O30</f>
+        <f t="shared" ref="S13:S14" si="17">T13</f>
         <v>0</v>
       </c>
       <c r="T13">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="T13:T14" si="18">U13</f>
         <v>0</v>
       </c>
       <c r="U13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="U13:U14" si="19">V13</f>
         <v>0</v>
       </c>
       <c r="V13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="V13:V14" si="20">W13</f>
         <v>0</v>
       </c>
       <c r="W13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="W13:W14" si="21">X13</f>
         <v>0</v>
       </c>
       <c r="X13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="X13:X14" si="22">Y13</f>
         <v>0</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Y13:Y14" si="23">Z13</f>
         <v>0</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Z13:Z14" si="24">AA13</f>
         <v>0</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AA13:AA14" si="25">AB13</f>
         <v>0</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AB13:AB14" si="26">AC13</f>
         <v>0</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AC13:AC14" si="27">AD13</f>
         <v>0</v>
       </c>
       <c r="AD13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AD13:AD14" si="28">AE13</f>
         <v>0</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AE13:AE14" si="29">AF13</f>
         <v>0</v>
       </c>
       <c r="AF13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AF13:AF14" si="30">AG13</f>
         <v>0</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AG13:AG14" si="31">AH13</f>
         <v>0</v>
       </c>
       <c r="AH13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AH13:AH14" si="32">AI13</f>
         <v>0</v>
       </c>
       <c r="AI13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AI13:AI14" si="33">AJ13</f>
         <v>0</v>
       </c>
       <c r="AJ13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AJ13:AJ14" si="34">AK13</f>
         <v>0</v>
       </c>
       <c r="AK13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AK13:AK14" si="35">AL13</f>
         <v>0</v>
       </c>
       <c r="AL13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AL13:AL14" si="36">AM13</f>
         <v>0</v>
       </c>
       <c r="AM13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AM13:AM14" si="37">AN13</f>
         <v>0</v>
       </c>
     </row>
@@ -4977,156 +4528,118 @@
         <v>31</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
-        <v>1.0728312983511656E-4</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
-        <v>1.0728312983511656E-4</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>1.0728312983511656E-4</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
-        <v>1.0728312983511656E-4</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <f>'Technologies to power CCS'!B31</f>
-        <v>1.0728312983511656E-4</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <f>'Technologies to power CCS'!C31</f>
-        <v>1.481058739776992E-4</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <f>'Technologies to power CCS'!D31</f>
-        <v>1.861401877596074E-4</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <f>'Technologies to power CCS'!E31</f>
-        <v>2.2193262480603088E-4</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <f>'Technologies to power CCS'!F31</f>
-        <v>2.1525763325093273E-4</v>
+        <v>0</v>
       </c>
       <c r="K14">
-        <f>'Technologies to power CCS'!G31</f>
-        <v>2.1128641310043373E-4</v>
+        <v>0</v>
       </c>
       <c r="L14">
-        <f>'Technologies to power CCS'!H31</f>
-        <v>2.0855474895847758E-4</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <f>'Technologies to power CCS'!I31</f>
-        <v>2.0626790405407189E-4</v>
+        <v>0</v>
       </c>
       <c r="N14">
-        <f>'Technologies to power CCS'!J31</f>
-        <v>2.0314930173522008E-4</v>
+        <v>0</v>
       </c>
       <c r="O14">
-        <f>'Technologies to power CCS'!K31</f>
-        <v>1.9712870217559122E-4</v>
+        <v>0</v>
       </c>
       <c r="P14">
-        <f>'Technologies to power CCS'!L31</f>
-        <v>1.9224351255042548E-4</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <f>'Technologies to power CCS'!M31</f>
-        <v>1.88979901609504E-4</v>
+        <v>0</v>
       </c>
       <c r="R14">
-        <f>'Technologies to power CCS'!N31</f>
-        <v>1.8501228777610494E-4</v>
+        <v>0</v>
       </c>
       <c r="S14">
-        <f>'Technologies to power CCS'!O31</f>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="T14">
-        <f t="shared" si="3"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="U14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="V14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="W14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="X14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AF14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AH14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AI14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AJ14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AK14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AL14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
       <c r="AM14">
-        <f t="shared" si="1"/>
-        <v>2.1380291675640448E-4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>